<commit_message>
new location for the key spreadsheet - pulling from box sync now, will remove later.
</commit_message>
<xml_diff>
--- a/spreadsheets/key.xlsx
+++ b/spreadsheets/key.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\astarke\Documents\tidalCulvert_datasheet\spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\astarke\AppData\Local\Box\Box Edit\Documents\S1hbSucr8kC0hi54HIH3ig==\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{01B7602E-F96B-43F0-A7E1-B0FB0734ECCB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EC63CF42-93DD-447F-ADE5-BD7DD366CFF7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13530" xr2:uid="{9670CEC8-E083-48E7-8065-1DD667B6ADBE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="91">
   <si>
     <t>Sheet</t>
   </si>
@@ -195,10 +196,109 @@
     <t>AC48</t>
   </si>
   <si>
-    <t>headwallMat_up</t>
-  </si>
-  <si>
     <t>B61</t>
+  </si>
+  <si>
+    <t>CrossingConditionEval</t>
+  </si>
+  <si>
+    <t>N12</t>
+  </si>
+  <si>
+    <t>TidalRngRatio</t>
+  </si>
+  <si>
+    <t>N14</t>
+  </si>
+  <si>
+    <t>Assessment</t>
+  </si>
+  <si>
+    <t>GeneralAssessmentNotes</t>
+  </si>
+  <si>
+    <t>Municipality</t>
+  </si>
+  <si>
+    <t>TidePredictTimeHigh</t>
+  </si>
+  <si>
+    <t>TidePredictTimeLow</t>
+  </si>
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>TidePredictElevationHigh</t>
+  </si>
+  <si>
+    <t>TidePredictElevationLow</t>
+  </si>
+  <si>
+    <t>G11</t>
+  </si>
+  <si>
+    <t>AA13</t>
+  </si>
+  <si>
+    <t>AE13</t>
+  </si>
+  <si>
+    <t>AA14</t>
+  </si>
+  <si>
+    <t>AE14</t>
+  </si>
+  <si>
+    <t>LowTidePerch_upStream</t>
+  </si>
+  <si>
+    <t>LowTidePerch_dwnStream</t>
+  </si>
+  <si>
+    <t>HighTidePerch_upStream</t>
+  </si>
+  <si>
+    <t>HighTidePerch_dwnStream</t>
+  </si>
+  <si>
+    <t>Z55</t>
+  </si>
+  <si>
+    <t>AD55</t>
+  </si>
+  <si>
+    <t>Z56</t>
+  </si>
+  <si>
+    <t>AD56</t>
+  </si>
+  <si>
+    <t>HeadwallMaterial_upStream</t>
+  </si>
+  <si>
+    <t>HeadwallCondition_upStream</t>
+  </si>
+  <si>
+    <t>I62</t>
+  </si>
+  <si>
+    <t>WindwallCondition_upStream</t>
+  </si>
+  <si>
+    <t>ScourSeverity_upStream</t>
+  </si>
+  <si>
+    <t>ScourStructure_upStream</t>
+  </si>
+  <si>
+    <t>U62</t>
+  </si>
+  <si>
+    <t>Y61</t>
+  </si>
+  <si>
+    <t>AD62</t>
   </si>
 </sst>
 </file>
@@ -596,10 +696,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35757D44-DE7F-4365-9039-1ED3324740B0}">
-  <dimension ref="A1:F26"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:XFD40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,83 +799,83 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>31</v>
@@ -782,13 +883,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>28</v>
+        <v>73</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>31</v>
@@ -964,22 +1065,285 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C26" s="7" t="s">
+      <c r="D35" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>31</v>
+      <c r="B40" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A7C71DF6-CDFC-4B34-9863-2616E299EC64}">
+          <x14:formula1>
+            <xm:f>Sheet2!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B39 B40:B1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43E65516-7B9A-48D9-9BD9-1A657BEF9A4A}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{F3C0C286-6761-4D3E-AC84-79E26651621F}">
-      <formula1>$B$4:$B$7</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A3" xr:uid="{B23AF559-9DFC-4882-81DE-2BC864067AA6}">
+      <formula1>$B$4:$B$18</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>